<commit_message>
updated and ran the orleikon website
</commit_message>
<xml_diff>
--- a/batch1.xlsx
+++ b/batch1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DCMME_git\Web-scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC10367-F73C-4C6F-AD3B-95EE5009AF24}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F944BA-D3B0-4A95-AC2B-F79AE438B940}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9402" xr2:uid="{3BB731C8-CC94-416A-9520-170C1B6F9CC4}"/>
   </bookViews>
@@ -74,10 +74,10 @@
     <t>Comments/ vamsi</t>
   </si>
   <si>
-    <t>https://www.grandindustrial.com/</t>
-  </si>
-  <si>
     <t>http://www.hscast.com/</t>
+  </si>
+  <si>
+    <t>https://www.oerlikon.com/fairfield/en/</t>
   </si>
 </sst>
 </file>
@@ -205,6 +205,96 @@
   <dxfs count="11">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -222,104 +312,14 @@
       <fill>
         <patternFill patternType="none">
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{A58DFD45-DC68-4BB2-AE8A-FB4D9B118255}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -633,7 +633,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -712,21 +712,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>